<commit_message>
SSDM-12286 Added export support for parents and children of samples.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF048935-836E-7C42-87B1-FC4A6ECD341E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE9C85D-663D-E840-9705-7E6B0C73B837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1060" windowWidth="27320" windowHeight="16940" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Code</t>
   </si>
@@ -102,6 +102,32 @@
   </si>
   <si>
     <t>/ELN_SETTINGS/STORAGES/DEFAULT_STORAGE</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/STORAGES/CHILD_1</t>
+  </si>
+  <si>
+    <t>CHILD_1</t>
+  </si>
+  <si>
+    <t>Child 1</t>
+  </si>
+  <si>
+    <t>CHILD_2</t>
+  </si>
+  <si>
+    <t>Child 2</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/STORAGES/CHILD_1
+/ELN_SETTINGS/STORAGES/CHILD_2</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/STORAGES/BENCH
+/ELN_SETTINGS/STORAGES/DEFAULT_STORAGE</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/STORAGES/CHILD_2</t>
   </si>
 </sst>
 </file>
@@ -184,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -207,7 +233,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,18 +553,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7C1F4F-E040-CE4F-B58F-ED261D5355F7}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,7 +633,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -617,7 +653,9 @@
         <v>0</v>
       </c>
       <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
@@ -625,7 +663,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="36" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -644,11 +682,72 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="I6" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="J6" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="9">
         <v>1111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>